<commit_message>
feat(ui): Introduce typed UI state management for trade functionality
- Added `ui/state` folder with typed state containers for trade operations.
- Implemented `TradeTransaction`, `TradeTeamPackage`, `TradeSlot`, and `TradeState` classes in `trade_state.py`.
- Created `README.md` for documentation on the `ui/state` folder responsibilities and structure.
- Refactored `TeamShuffleWindow` to use Dear PyGui for UI components, replacing Tkinter.
- Updated `teams_screen.py` to utilize Dear PyGui for team management interface.
- Introduced `trade_players.py` for managing player trades within the UI.
- Enhanced theme management in `theme.py` for Dear PyGui compatibility.
- Removed obsolete Tkinter widget helpers in `widgets.py` and replaced with Dear PyGui equivalents.
</commit_message>
<xml_diff>
--- a/nba2k26_editor/Offsets/ImportPlayers.xlsx
+++ b/nba2k26_editor/Offsets/ImportPlayers.xlsx
@@ -19,6 +19,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stats" sheetId="10" state="visible" r:id="rId10"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Contracts" sheetId="11" state="visible" r:id="rId11"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Edit" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Signature" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -436,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DN1"/>
+  <dimension ref="A1:DV1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,580 +458,620 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>ARM_SCALE</t>
+          <t>Appearance Data</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Arm Scale</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Audio Signature ID</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Average Percent</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Birth Day</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Birth Month</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Birth Year</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>BODYLENGTH</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>BODY_SHAPE</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Boom Percentage</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>BOOM_OR_BUST</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Boom Percentage</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Bust Percentage</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>CAREERENDINGINJURYALLOWED</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>College</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>CONTRACT_TEAM</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Contract Team</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Created Player Nickname</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Current Team</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Current Team Address</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Custom Age at Set Year</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Dominant Hand</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>DRAFTED_TEAM</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Dominant Dunk Hand</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Draft Pick Number</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Drafted Team</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Drafted Year</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>DRAFTPICK</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>DRAFTROUND</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>DRAFTYEAR</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Dunk Hand</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>EYE_COLOR</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Face ID</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Financial Security</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>First Name</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>FIRSTNAMESHOWCASE</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Force Non Starter</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>G-LEAGUE_TEAM_ID</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>GENDER</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>G-LEAGUE_TEAM_ID</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Gender Created Player</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>HADIMPORTANTINJURY</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>HAIR_LENGTH</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>HAND_SCALE</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Headshot ID</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Height</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>Height (cm)</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>HOMETOWN_TEAM</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Hometown Team 1</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>Hometown Team 2</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Injury 1 Duration</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Injury 1 Status</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Injury 1 Type</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>Injury 2 Duration (Days)</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>Injury 2 Status</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>Injury 2 Type</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>INJURY1BODY</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>INJURY1DAY</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>Injury 1 Duration</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>Injury 1 Status</t>
-        </is>
-      </c>
-      <c r="AS1" s="1" t="inlineStr">
-        <is>
-          <t>Injury 1 Type</t>
-        </is>
-      </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>INJURY2BODY</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>INJURY2DAY</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
-        <is>
-          <t>Injury 2 Status</t>
-        </is>
-      </c>
-      <c r="AW1" s="1" t="inlineStr">
-        <is>
-          <t>Injury 2 Type</t>
-        </is>
-      </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>Is Active</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>Is Draft Prospect</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>Is G-League Send Down</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>Is Generated</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>Is Hidden</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>Is Historic</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>Is Injury 1 Type Left Body</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>Is Injury 2 Type Left Body</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
         <is>
           <t>IS_DLEAGUE</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BL1" s="1" t="inlineStr">
         <is>
           <t>IS_DRAFTED_IN_TEAM_EXPANSION</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
-        <is>
-          <t>Is Draft Prospect</t>
-        </is>
-      </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BM1" s="1" t="inlineStr">
         <is>
           <t>IS_ELIGIBLE_FOR_FANTASY_DRAFT</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
-        <is>
-          <t>Is Generated</t>
-        </is>
-      </c>
-      <c r="BD1" s="1" t="inlineStr">
-        <is>
-          <t>Is G-League Send Down</t>
-        </is>
-      </c>
-      <c r="BE1" s="1" t="inlineStr">
-        <is>
-          <t>Is Hidden</t>
-        </is>
-      </c>
-      <c r="BF1" s="1" t="inlineStr">
-        <is>
-          <t>Is Historic</t>
-        </is>
-      </c>
-      <c r="BG1" s="1" t="inlineStr">
-        <is>
-          <t>Is Injury 1 Type Left Body</t>
-        </is>
-      </c>
-      <c r="BH1" s="1" t="inlineStr">
-        <is>
-          <t>Is Injury 2 Type Left Body</t>
-        </is>
-      </c>
-      <c r="BI1" s="1" t="inlineStr">
+      <c r="BN1" s="1" t="inlineStr">
         <is>
           <t>IS_PROTECTED_IN_TEAM_EXTENSION_DRAFT</t>
         </is>
       </c>
-      <c r="BJ1" s="1" t="inlineStr">
+      <c r="BO1" s="1" t="inlineStr">
         <is>
           <t>IS_SUMMER_LEAGUE_ATTENDEE</t>
         </is>
       </c>
-      <c r="BK1" s="1" t="inlineStr">
+      <c r="BP1" s="1" t="inlineStr">
         <is>
           <t>Jersey Nick Name</t>
         </is>
       </c>
-      <c r="BL1" s="1" t="inlineStr">
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>Jersey Number</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
         <is>
           <t>Last Name</t>
         </is>
       </c>
-      <c r="BM1" s="1" t="inlineStr">
+      <c r="BS1" s="1" t="inlineStr">
         <is>
           <t>LOWER_SCALE</t>
         </is>
       </c>
-      <c r="BN1" s="1" t="inlineStr">
-        <is>
-          <t>LOYALITY</t>
-        </is>
-      </c>
-      <c r="BO1" s="1" t="inlineStr">
+      <c r="BT1" s="1" t="inlineStr">
         <is>
           <t>Loyalty</t>
         </is>
       </c>
-      <c r="BP1" s="1" t="inlineStr">
+      <c r="BU1" s="1" t="inlineStr">
         <is>
           <t>MAKE_A_COACH</t>
         </is>
       </c>
-      <c r="BQ1" s="1" t="inlineStr">
+      <c r="BV1" s="1" t="inlineStr">
         <is>
           <t>Maximum Potential</t>
         </is>
       </c>
-      <c r="BR1" s="1" t="inlineStr">
+      <c r="BW1" s="1" t="inlineStr">
         <is>
           <t>Minimum Potential</t>
         </is>
       </c>
-      <c r="BS1" s="1" t="inlineStr">
+      <c r="BX1" s="1" t="inlineStr">
         <is>
           <t>MURAL_ID</t>
         </is>
       </c>
-      <c r="BT1" s="1" t="inlineStr">
+      <c r="BY1" s="1" t="inlineStr">
         <is>
           <t>MURAL_TEAM</t>
         </is>
       </c>
-      <c r="BU1" s="1" t="inlineStr">
+      <c r="BZ1" s="1" t="inlineStr">
         <is>
           <t>MUST_RETIRE_NEXT_YEAR</t>
         </is>
       </c>
-      <c r="BV1" s="1" t="inlineStr">
+      <c r="CA1" s="1" t="inlineStr">
         <is>
           <t>MYTEAM_DUPLICATE_ID</t>
         </is>
       </c>
-      <c r="BW1" s="1" t="inlineStr">
+      <c r="CB1" s="1" t="inlineStr">
         <is>
           <t>Name Order</t>
         </is>
       </c>
-      <c r="BX1" s="1" t="inlineStr">
+      <c r="CC1" s="1" t="inlineStr">
         <is>
           <t>NAMESID</t>
         </is>
       </c>
-      <c r="BY1" s="1" t="inlineStr">
+      <c r="CD1" s="1" t="inlineStr">
+        <is>
+          <t>Neck Length</t>
+        </is>
+      </c>
+      <c r="CE1" s="1" t="inlineStr">
         <is>
           <t>NECK_HEAD_SCALE</t>
         </is>
       </c>
-      <c r="BZ1" s="1" t="inlineStr">
+      <c r="CF1" s="1" t="inlineStr">
         <is>
           <t>Nick Name</t>
         </is>
       </c>
-      <c r="CA1" s="1" t="inlineStr">
+      <c r="CG1" s="1" t="inlineStr">
         <is>
           <t>NICKNAME1</t>
         </is>
       </c>
-      <c r="CB1" s="1" t="inlineStr">
-        <is>
-          <t>Created Player Nickname</t>
-        </is>
-      </c>
-      <c r="CC1" s="1" t="inlineStr">
-        <is>
-          <t>Jersey Number</t>
-        </is>
-      </c>
-      <c r="CD1" s="1" t="inlineStr">
+      <c r="CH1" s="1" t="inlineStr">
         <is>
           <t>ORIGINALINJURY1TYPE</t>
         </is>
       </c>
-      <c r="CE1" s="1" t="inlineStr">
+      <c r="CI1" s="1" t="inlineStr">
         <is>
           <t>ORIGINALINJURY2TYPE</t>
         </is>
       </c>
-      <c r="CF1" s="1" t="inlineStr">
-        <is>
-          <t>Peak End</t>
-        </is>
-      </c>
-      <c r="CG1" s="1" t="inlineStr">
+      <c r="CJ1" s="1" t="inlineStr">
         <is>
           <t>Peak End Age</t>
         </is>
       </c>
-      <c r="CH1" s="1" t="inlineStr">
-        <is>
-          <t>Peak Start</t>
-        </is>
-      </c>
-      <c r="CI1" s="1" t="inlineStr">
+      <c r="CK1" s="1" t="inlineStr">
         <is>
           <t>Peak Start Age</t>
         </is>
       </c>
-      <c r="CJ1" s="1" t="inlineStr">
+      <c r="CL1" s="1" t="inlineStr">
+        <is>
+          <t>PEAKEND</t>
+        </is>
+      </c>
+      <c r="CM1" s="1" t="inlineStr">
+        <is>
+          <t>PEAKSTART</t>
+        </is>
+      </c>
+      <c r="CN1" s="1" t="inlineStr">
         <is>
           <t>PERSONALITY</t>
         </is>
       </c>
-      <c r="CK1" s="1" t="inlineStr">
+      <c r="CO1" s="1" t="inlineStr">
         <is>
           <t>PHOTOID</t>
         </is>
       </c>
-      <c r="CL1" s="1" t="inlineStr">
+      <c r="CP1" s="1" t="inlineStr">
         <is>
           <t>Play For Winner</t>
         </is>
       </c>
-      <c r="CM1" s="1" t="inlineStr">
+      <c r="CQ1" s="1" t="inlineStr">
         <is>
           <t>Play Initiator</t>
         </is>
       </c>
-      <c r="CN1" s="1" t="inlineStr">
-        <is>
-          <t>Playtype 1</t>
-        </is>
-      </c>
-      <c r="CO1" s="1" t="inlineStr">
-        <is>
-          <t>Playtype 2</t>
-        </is>
-      </c>
-      <c r="CP1" s="1" t="inlineStr">
-        <is>
-          <t>Playtype 3</t>
-        </is>
-      </c>
-      <c r="CQ1" s="1" t="inlineStr">
-        <is>
-          <t>Playtype 4</t>
-        </is>
-      </c>
       <c r="CR1" s="1" t="inlineStr">
         <is>
+          <t>Play Type 1</t>
+        </is>
+      </c>
+      <c r="CS1" s="1" t="inlineStr">
+        <is>
+          <t>Play Type 2</t>
+        </is>
+      </c>
+      <c r="CT1" s="1" t="inlineStr">
+        <is>
+          <t>Play Type 3</t>
+        </is>
+      </c>
+      <c r="CU1" s="1" t="inlineStr">
+        <is>
+          <t>Play Type 4</t>
+        </is>
+      </c>
+      <c r="CV1" s="1" t="inlineStr">
+        <is>
+          <t>Player Type</t>
+        </is>
+      </c>
+      <c r="CW1" s="1" t="inlineStr">
+        <is>
           <t>Portrait ID</t>
         </is>
       </c>
-      <c r="CS1" s="1" t="inlineStr">
-        <is>
-          <t>Portrait Team 1</t>
-        </is>
-      </c>
-      <c r="CT1" s="1" t="inlineStr">
+      <c r="CX1" s="1" t="inlineStr">
+        <is>
+          <t>Portrait Team  #1</t>
+        </is>
+      </c>
+      <c r="CY1" s="1" t="inlineStr">
         <is>
           <t>Portrait Team 2</t>
         </is>
       </c>
-      <c r="CU1" s="1" t="inlineStr">
+      <c r="CZ1" s="1" t="inlineStr">
         <is>
           <t>Position</t>
         </is>
       </c>
-      <c r="CV1" s="1" t="inlineStr">
+      <c r="DA1" s="1" t="inlineStr">
         <is>
           <t>PREVIOUS_TEAM</t>
         </is>
       </c>
-      <c r="CW1" s="1" t="inlineStr">
+      <c r="DB1" s="1" t="inlineStr">
         <is>
           <t>QUALIFIESFORWORLDTEAM</t>
         </is>
       </c>
-      <c r="CX1" s="1" t="inlineStr">
+      <c r="DC1" s="1" t="inlineStr">
         <is>
           <t>RECENT_DRAFT_SIGNING</t>
         </is>
       </c>
-      <c r="CY1" s="1" t="inlineStr">
+      <c r="DD1" s="1" t="inlineStr">
         <is>
           <t>RETIREMENT</t>
         </is>
       </c>
-      <c r="CZ1" s="1" t="inlineStr">
+      <c r="DE1" s="1" t="inlineStr">
         <is>
           <t>Round Drafted</t>
         </is>
       </c>
-      <c r="DA1" s="1" t="inlineStr">
-        <is>
-          <t>Position 2</t>
-        </is>
-      </c>
-      <c r="DB1" s="1" t="inlineStr">
+      <c r="DF1" s="1" t="inlineStr">
+        <is>
+          <t>Secondary Position</t>
+        </is>
+      </c>
+      <c r="DG1" s="1" t="inlineStr">
+        <is>
+          <t>Shoulder Length</t>
+        </is>
+      </c>
+      <c r="DH1" s="1" t="inlineStr">
         <is>
           <t>SHOULDERWIDTH</t>
         </is>
       </c>
-      <c r="DC1" s="1" t="inlineStr">
-        <is>
-          <t>*Signature ID</t>
-        </is>
-      </c>
-      <c r="DD1" s="1" t="inlineStr">
+      <c r="DI1" s="1" t="inlineStr">
         <is>
           <t>SKINCOLOR</t>
         </is>
       </c>
-      <c r="DE1" s="1" t="inlineStr">
+      <c r="DJ1" s="1" t="inlineStr">
         <is>
           <t>SKINTYPE</t>
         </is>
       </c>
-      <c r="DF1" s="1" t="inlineStr">
+      <c r="DK1" s="1" t="inlineStr">
         <is>
           <t>Special Case Name</t>
         </is>
       </c>
-      <c r="DG1" s="1" t="inlineStr">
+      <c r="DL1" s="1" t="inlineStr">
         <is>
           <t>THIRD_POSITION</t>
         </is>
       </c>
-      <c r="DH1" s="1" t="inlineStr">
+      <c r="DM1" s="1" t="inlineStr">
+        <is>
+          <t>Trunk Length</t>
+        </is>
+      </c>
+      <c r="DN1" s="1" t="inlineStr">
         <is>
           <t>TYPE</t>
         </is>
       </c>
-      <c r="DI1" s="1" t="inlineStr">
+      <c r="DO1" s="1" t="inlineStr">
         <is>
           <t>UNIQUEID</t>
         </is>
       </c>
-      <c r="DJ1" s="1" t="inlineStr">
+      <c r="DP1" s="1" t="inlineStr">
+        <is>
+          <t>Used Retirement Grace</t>
+        </is>
+      </c>
+      <c r="DQ1" s="1" t="inlineStr">
         <is>
           <t>VOICETYPE</t>
         </is>
       </c>
-      <c r="DK1" s="1" t="inlineStr">
+      <c r="DR1" s="1" t="inlineStr">
         <is>
           <t>Was Drafted</t>
         </is>
       </c>
-      <c r="DL1" s="1" t="inlineStr">
+      <c r="DS1" s="1" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="DM1" s="1" t="inlineStr">
+      <c r="DT1" s="1" t="inlineStr">
+        <is>
+          <t>Weight (kg)</t>
+        </is>
+      </c>
+      <c r="DU1" s="1" t="inlineStr">
         <is>
           <t>Wingspan</t>
         </is>
       </c>
-      <c r="DN1" s="1" t="inlineStr">
+      <c r="DV1" s="1" t="inlineStr">
         <is>
           <t>Years Pro</t>
         </is>
@@ -1047,7 +1088,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BQ1"/>
+  <dimension ref="A1:AZ1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1058,347 +1099,262 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>3PT_FIELD_GOALS_ATTEMPTED#CAREER</t>
+          <t>All Star West</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>3PT_FIELD_GOALS_ATTEMPTED#SEASON</t>
+          <t>All-Defense Team</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>3PT_FIELD_GOALS_MADE#CAREER</t>
+          <t>All-NBA Team</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>3PT_FIELD_GOALS_MADE#SEASON</t>
+          <t>All-Rookie Team</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>ASSISTS#CAREER</t>
+          <t>All-Star East</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>ASSISTS#SEASON</t>
+          <t>Assists</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>BLOCKS#CAREER</t>
+          <t>Assists#Career</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>BLOCKS#SEASON</t>
+          <t>Blocks</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>Blocks#Career</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Championship</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>Current Team</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>CURRENT_YEAR_STATS</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>DEFENSIVE_REBOUNDS#CAREER</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>DEFENSIVE_REBOUNDS#SEASON</t>
-        </is>
-      </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>FIELD_GOALS_ATTEMPTED#CAREER</t>
+          <t>Defensive Player Of The Year</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>FIELD_GOALS_ATTEMPTED#SEASON</t>
+          <t>Defensive Rebounds</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>FIELD_GOALS_MADE#CAREER</t>
+          <t>Defensive Rebounds#Career</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>FIELD_GOALS_MADE#SEASON</t>
+          <t>Double Doubles</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>FREE_THROWS_ATTEMPTED#CAREER</t>
+          <t>Field Goals Attempted</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>FREE_THROWS_ATTEMPTED#SEASON</t>
+          <t>Field Goals Attempted#Career</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>FREE_THROWS_MADE#CAREER</t>
+          <t>Field Goals Made</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>FREE_THROWS_MADE#SEASON</t>
+          <t>Field Goals Made#Career</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
+          <t>Finals MVP</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Fouls</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Free Throws Attempted</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Free Throws Attempted#Career</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Free Throws Made</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Free Throws Made#Career</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Games Played</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Games Started</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
           <t>Is Used</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>MINUTES_PLAYED#CAREER</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>MINUTES_PLAYED#SEASON</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>OFFENSIVE_REBOUNDS#CAREER</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>OFFENSIVE_REBOUNDS#SEASON</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>Player Stat ID 18</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>Player Stat ID 19</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>Player Stat ID 20</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>Player Stat ID 21</t>
-        </is>
-      </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>Player Stat ID 22</t>
+          <t>Jersey Number</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>Player Stat ID 23</t>
+          <t>Minutes</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>Player Stat ID 24</t>
+          <t>Minutes Played#Career</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>Player Stat ID 25</t>
+          <t>Most Improved Player</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>Player Stat ID 26</t>
+          <t>Most Valuable Player</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>Player Stat ID 27</t>
+          <t>Offensive Rebounds</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>Player Stat ID 28</t>
+          <t>Offensive Rebounds#Career</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>Player Stat ID 29</t>
+          <t>Overall</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>Player Stat ID 30</t>
+          <t>Points</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>Player Stat ID 31</t>
+          <t>Points#Career</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>POINTS#CAREER</t>
+          <t>Previous Team</t>
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
-          <t>POINTS#SEASON</t>
+          <t>Rebounds#Career</t>
         </is>
       </c>
       <c r="AP1" s="1" t="inlineStr">
         <is>
-          <t>STATS_ID#1</t>
+          <t>Rookie Of The Year</t>
         </is>
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
-          <t>STATS_ID#10</t>
+          <t>Sixth Man</t>
         </is>
       </c>
       <c r="AR1" s="1" t="inlineStr">
         <is>
-          <t>STATS_ID#11</t>
+          <t>Steals</t>
         </is>
       </c>
       <c r="AS1" s="1" t="inlineStr">
         <is>
-          <t>STATS_ID#12</t>
+          <t>Steals#Career</t>
         </is>
       </c>
       <c r="AT1" s="1" t="inlineStr">
         <is>
-          <t>STATS_ID#13</t>
+          <t>Three Pointers Attempted</t>
         </is>
       </c>
       <c r="AU1" s="1" t="inlineStr">
         <is>
-          <t>STATS_ID#14</t>
+          <t>Three Pointers Attempted#Career</t>
         </is>
       </c>
       <c r="AV1" s="1" t="inlineStr">
         <is>
-          <t>STATS_ID#15</t>
+          <t>Three Pointers Made</t>
         </is>
       </c>
       <c r="AW1" s="1" t="inlineStr">
         <is>
-          <t>STATS_ID#16</t>
+          <t>Three Pointers Made#Career</t>
         </is>
       </c>
       <c r="AX1" s="1" t="inlineStr">
         <is>
-          <t>STATS_ID#17</t>
+          <t>Total +/-</t>
         </is>
       </c>
       <c r="AY1" s="1" t="inlineStr">
         <is>
-          <t>STATS_ID#18</t>
+          <t>Triple Doubles</t>
         </is>
       </c>
       <c r="AZ1" s="1" t="inlineStr">
         <is>
-          <t>STATS_ID#19</t>
-        </is>
-      </c>
-      <c r="BA1" s="1" t="inlineStr">
-        <is>
-          <t>STATS_ID#2</t>
-        </is>
-      </c>
-      <c r="BB1" s="1" t="inlineStr">
-        <is>
-          <t>STATS_ID#20</t>
-        </is>
-      </c>
-      <c r="BC1" s="1" t="inlineStr">
-        <is>
-          <t>STATS_ID#21</t>
-        </is>
-      </c>
-      <c r="BD1" s="1" t="inlineStr">
-        <is>
-          <t>STATS_ID#22</t>
-        </is>
-      </c>
-      <c r="BE1" s="1" t="inlineStr">
-        <is>
-          <t>STATS_ID#23</t>
-        </is>
-      </c>
-      <c r="BF1" s="1" t="inlineStr">
-        <is>
-          <t>STATS_ID#24</t>
-        </is>
-      </c>
-      <c r="BG1" s="1" t="inlineStr">
-        <is>
-          <t>STATS_ID#3</t>
-        </is>
-      </c>
-      <c r="BH1" s="1" t="inlineStr">
-        <is>
-          <t>STATS_ID#4</t>
-        </is>
-      </c>
-      <c r="BI1" s="1" t="inlineStr">
-        <is>
-          <t>STATS_ID#5</t>
-        </is>
-      </c>
-      <c r="BJ1" s="1" t="inlineStr">
-        <is>
-          <t>STATS_ID#6</t>
-        </is>
-      </c>
-      <c r="BK1" s="1" t="inlineStr">
-        <is>
-          <t>STATS_ID#7</t>
-        </is>
-      </c>
-      <c r="BL1" s="1" t="inlineStr">
-        <is>
-          <t>STATS_ID#8</t>
-        </is>
-      </c>
-      <c r="BM1" s="1" t="inlineStr">
-        <is>
-          <t>STATS_ID#9</t>
-        </is>
-      </c>
-      <c r="BN1" s="1" t="inlineStr">
-        <is>
-          <t>STEALS#CAREER</t>
-        </is>
-      </c>
-      <c r="BO1" s="1" t="inlineStr">
-        <is>
-          <t>STEALS#SEASON</t>
-        </is>
-      </c>
-      <c r="BP1" s="1" t="inlineStr">
-        <is>
-          <t>TOTAL_REBOUNDS#CAREER</t>
-        </is>
-      </c>
-      <c r="BQ1" s="1" t="inlineStr">
-        <is>
-          <t>TOTAL_REBOUNDS#SEASON</t>
+          <t>Turnovers</t>
         </is>
       </c>
     </row>
@@ -1413,7 +1369,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1424,97 +1380,102 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Bird Years</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Contract Thought</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>CONTRACT_OPTION</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>CONTRACT_TYPE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>EURO-STASH_YEARS_LEFT</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Extension Length</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Extension No Trade</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Extension Option</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Free Agency Type</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Option</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Original Contract Length</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>Two-Way NBA Days Left</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>BIRD_YEARS</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>CONTRACT_OPTION</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>CONTRACT_THOUGHT</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>CONTRACT_TYPE</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>EURO-STASH_YEARS_LEFT</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>EXTENSION_LENGTH</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>EXTENSION_NO_TRADE</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>EXTENSION_OPTION</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>NO_TRADE</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>ORIGINAL_CONTRACT_YEARS</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Year 1</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Year 2</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Year 3</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Year 4</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Year 5</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Year 6</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>YEARS_LEFT_ON_CONTRACT</t>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Years Left</t>
         </is>
       </c>
     </row>
@@ -1719,13 +1680,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BG1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1736,7 +1697,33 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Three Point</t>
+          <t>NBA Jumpball Ritual</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BI1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>3pt Shot</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -1776,255 +1763,265 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>Defensive Consistency</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Defensive Rebound</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Draw Foul</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Driving Dunk</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Driving Layup</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Free Throws</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Hands</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Head Durability</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Help Defense IQ</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Hustle</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Intangibles</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Interior Defense</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>LATERAL_QUICKNESS</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Left Ankle Durability</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Left Elbow Durability</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Left Foot Durability</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Left Hand Durability</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Left Hip Durability</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Left Knee Durability</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Left Shoulder Durability</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>MAX_OVR</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Midrange Shot</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>MIN_OVR</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Miscanellous Durability</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Neck Durability</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Offensive Consistency</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Offensive Rebound</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Pass Accuracy</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Pass Perception</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Passing IQ</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Passing Vision</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Perimeter Defense</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>PICK_AND_ROLL_DEFENSIVE_IQ</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Post Fade</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Post Hook</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>Post Moves</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Potential</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Right Ankle Durability</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Right Elbow Durability</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>Right Foot Durability</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>Right Hand Durability</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>Right Hip Durability</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>Right Knee Durability</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>Right Shoulder Durability</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>Shot IQ</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
           <t>SHOT_CONTEST</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Defensive Consistency</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Defensive Rebound</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Draw Foul</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Driving Dunk</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Driving Layup</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Free Throw</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Hands</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Head Durability</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Help Defense IQ</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Hustle</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Intangibles</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Interior Defense</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Shot IQ</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>LATERAL_QUICKNESS</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Left Ankle Durability</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Left Elbow Durability</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>Left Foot Durability</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>Left Hip Durability</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>Left Knee Durability</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>Left Shoulder Durability</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>MAX_OVR</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>Mid Range</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>MIN_OVR</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>Misc Durability</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>Neck Durability</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>Offensive Consistency</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>Offensive Rebound</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>Passing Accuracy</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
-        <is>
-          <t>Passing IQ</t>
-        </is>
-      </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>Passing Perception</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>Passing Vision</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>Perimeter Defense</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>PICK_AND_ROLL_DEFENSIVE_IQ</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>Post Control</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>Post Fade</t>
-        </is>
-      </c>
-      <c r="AS1" s="1" t="inlineStr">
-        <is>
-          <t>Post Hook</t>
-        </is>
-      </c>
-      <c r="AT1" s="1" t="inlineStr">
-        <is>
-          <t>Potential</t>
-        </is>
-      </c>
-      <c r="AU1" s="1" t="inlineStr">
-        <is>
-          <t>Right Ankle Durability</t>
-        </is>
-      </c>
-      <c r="AV1" s="1" t="inlineStr">
-        <is>
-          <t>Right Elbow Durability</t>
-        </is>
-      </c>
-      <c r="AW1" s="1" t="inlineStr">
-        <is>
-          <t>Right Foot Durability</t>
-        </is>
-      </c>
-      <c r="AX1" s="1" t="inlineStr">
-        <is>
-          <t>Right Hip Durability</t>
-        </is>
-      </c>
-      <c r="AY1" s="1" t="inlineStr">
-        <is>
-          <t>Right Knee Durability</t>
-        </is>
-      </c>
-      <c r="AZ1" s="1" t="inlineStr">
-        <is>
-          <t>Right Shoulder Durability</t>
-        </is>
-      </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>Speed</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
-        <is>
-          <t>Speed With Ball</t>
-        </is>
-      </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>Speed with Ball</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>Stamina</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>Standing Dunk</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>Steal</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>Strength</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>Vertical</t>
         </is>
@@ -2041,7 +2038,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BW1"/>
+  <dimension ref="A1:CN1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2052,375 +2049,460 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Shot Three Right Center</t>
+          <t>Alley Oop Pass</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Shot Three Left Center</t>
+          <t>Attack Strong On Drive</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Block Shot</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Contest Shot</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Contested Jumper 3pt</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Contested Jumper Mid</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Contested Jumper Mid-Range</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Dish To Open Man</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Dribble Spin</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Drive</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Drive Pull Up 3pt</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Drive Pull Up Mid</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Drive Pull Up Mid-Range</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Drive Right</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Driving Behind The Back</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Driving Crossover</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Driving Dribble Hesitation</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Driving Dunk Tendency</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Driving In And Out</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Driving Layup Tendency</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Driving Step Back</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Euro Step Layup</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Flashy Dunk</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Flashy Pass</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Floater</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Foul</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Hard Foul</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Hop Step Layup</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Iso Vs Average Defender</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Iso Vs Elite Defender</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Iso Vs Good Defender</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Iso Vs Poor Defender</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>No Driving Dribble Move</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>No Setup Dribble</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Off Screen Drive</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Off Screen Shot 3pt</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Off Screen Shot Mid</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>On Ball Steal</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Pass Interception</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Play Discipline</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Post Aggressive Backdown</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Post Back Down</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>Post Drive</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Post Drop Step</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Post Fade Left</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Post Fade Right</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>Post Hook Left</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>Post Hook Right</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>Post Hop Shot Tendency</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>Post Hop Step</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>Post Shimmy Shot</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>Post Spin</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>Post Step Back Shot</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>Post Up</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>Post Up And Under</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>Putback</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>Putback Dunk</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>Roll Vs Pop</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>Setup With Hesitation</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>Setup With Sizeup</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>Shoot</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>Shoot From Post</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>Shot 3pt Right</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>Shot Close</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>Shot Close Middle</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>Shot Close Right</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>Shot Mid Center</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>Shot Mid Left Center</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>Shot Mid Right</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>Shot Three Left-Center</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>Shot Three Right-Center</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>Shot Under Basket</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>Spin Jumper Tendency</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>Spin Layup</t>
+        </is>
+      </c>
+      <c r="BX1" s="1" t="inlineStr">
+        <is>
+          <t>Spot Up Drive</t>
+        </is>
+      </c>
+      <c r="BY1" s="1" t="inlineStr">
+        <is>
+          <t>Spot Up Shot Mid</t>
+        </is>
+      </c>
+      <c r="BZ1" s="1" t="inlineStr">
+        <is>
           <t>Spot Up Shot Three</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Alley Oop Pass</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Attack Strong On Drive</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Block Tendency</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Shot Mid Right Center</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Shot Close Left</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Contested Jumper Three</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Contested Jumper Mid</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Crash</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Dish To Open Man</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Dribble Crossover</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Dribble Half Spin</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Drive</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Drive Pull Up Three</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Drive Pull Up Mid</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Drive Right</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Dribble Behind The Back</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Driving Dribble Hesitation</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Driving Dunk Tendency</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Driving In And Out</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Driving Layup Tendency</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Dribble Stepback</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Euro Step Layup</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>Flashy Dunk</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>Flashy Pass</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>Floater</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>Foul</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>Hard Foul</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>Hop Step Layup</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>Iso Vs Average Defender</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>Iso Vs Elite Defender</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>Iso Vs Good Defender</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>Iso Vs Poor Defender</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>Shot Mid Left Center</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>Shot Mid</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
-        <is>
-          <t>No Driving Dribble Move</t>
-        </is>
-      </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>No Setup Dribble Move</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>Off Screen Drive</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>Steal Tendency</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>Pass Interception</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>Play Discipline</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>Post Aggressive Backdown</t>
-        </is>
-      </c>
-      <c r="AS1" s="1" t="inlineStr">
-        <is>
-          <t>Post Back Down</t>
-        </is>
-      </c>
-      <c r="AT1" s="1" t="inlineStr">
-        <is>
-          <t>Post Drive</t>
-        </is>
-      </c>
-      <c r="AU1" s="1" t="inlineStr">
-        <is>
-          <t>Post Dropstep</t>
-        </is>
-      </c>
-      <c r="AV1" s="1" t="inlineStr">
-        <is>
-          <t>Post Fade Left</t>
-        </is>
-      </c>
-      <c r="AW1" s="1" t="inlineStr">
-        <is>
-          <t>Post Fade Right</t>
-        </is>
-      </c>
-      <c r="AX1" s="1" t="inlineStr">
-        <is>
-          <t>Post Hook Left</t>
-        </is>
-      </c>
-      <c r="AY1" s="1" t="inlineStr">
-        <is>
-          <t>Post Hook Right</t>
-        </is>
-      </c>
-      <c r="AZ1" s="1" t="inlineStr">
-        <is>
-          <t>Post Hop Step</t>
-        </is>
-      </c>
-      <c r="BA1" s="1" t="inlineStr">
-        <is>
-          <t>Post Spin</t>
-        </is>
-      </c>
-      <c r="BB1" s="1" t="inlineStr">
-        <is>
-          <t>Post Face Up</t>
-        </is>
-      </c>
-      <c r="BC1" s="1" t="inlineStr">
-        <is>
-          <t>Post Up And Under</t>
-        </is>
-      </c>
-      <c r="BD1" s="1" t="inlineStr">
-        <is>
-          <t>Putback Dunk</t>
-        </is>
-      </c>
-      <c r="BE1" s="1" t="inlineStr">
-        <is>
-          <t>Roll Vs Pop</t>
-        </is>
-      </c>
-      <c r="BF1" s="1" t="inlineStr">
-        <is>
-          <t>Setup With Hesitation</t>
-        </is>
-      </c>
-      <c r="BG1" s="1" t="inlineStr">
-        <is>
-          <t>Setup With Sizeup</t>
-        </is>
-      </c>
-      <c r="BH1" s="1" t="inlineStr">
-        <is>
-          <t>Shot Under Basket</t>
-        </is>
-      </c>
-      <c r="BI1" s="1" t="inlineStr">
-        <is>
-          <t>Spin Jumper</t>
-        </is>
-      </c>
-      <c r="BJ1" s="1" t="inlineStr">
-        <is>
-          <t>Spin Layup</t>
-        </is>
-      </c>
-      <c r="BK1" s="1" t="inlineStr">
-        <is>
-          <t>Spot Up Drive</t>
-        </is>
-      </c>
-      <c r="BL1" s="1" t="inlineStr">
+      <c r="CA1" s="1" t="inlineStr">
         <is>
           <t>Standing Dunk Tendency</t>
         </is>
       </c>
-      <c r="BM1" s="1" t="inlineStr">
-        <is>
-          <t>Stepback Jumper Three</t>
-        </is>
-      </c>
-      <c r="BN1" s="1" t="inlineStr">
-        <is>
-          <t>Step Back Jumper Mid</t>
-        </is>
-      </c>
-      <c r="BO1" s="1" t="inlineStr">
-        <is>
-          <t>Step Through</t>
-        </is>
-      </c>
-      <c r="BP1" s="1" t="inlineStr">
+      <c r="CB1" s="1" t="inlineStr">
+        <is>
+          <t>Step Through Shot</t>
+        </is>
+      </c>
+      <c r="CC1" s="1" t="inlineStr">
+        <is>
+          <t>Stepback Jumper 3pt</t>
+        </is>
+      </c>
+      <c r="CD1" s="1" t="inlineStr">
+        <is>
+          <t>Stepback Jumper Mid</t>
+        </is>
+      </c>
+      <c r="CE1" s="1" t="inlineStr">
+        <is>
+          <t>Stepback Jumper Mid-Range</t>
+        </is>
+      </c>
+      <c r="CF1" s="1" t="inlineStr">
         <is>
           <t>Take Charge</t>
         </is>
       </c>
-      <c r="BQ1" s="1" t="inlineStr">
+      <c r="CG1" s="1" t="inlineStr">
         <is>
           <t>Touches</t>
         </is>
       </c>
-      <c r="BR1" s="1" t="inlineStr">
-        <is>
-          <t>Transition Pull Up Three</t>
-        </is>
-      </c>
-      <c r="BS1" s="1" t="inlineStr">
+      <c r="CH1" s="1" t="inlineStr">
+        <is>
+          <t>Transition Pull Up 3pt</t>
+        </is>
+      </c>
+      <c r="CI1" s="1" t="inlineStr">
         <is>
           <t>Transition Spot Up</t>
         </is>
       </c>
-      <c r="BT1" s="1" t="inlineStr">
+      <c r="CJ1" s="1" t="inlineStr">
         <is>
           <t>Triple Threat Idle</t>
         </is>
       </c>
-      <c r="BU1" s="1" t="inlineStr">
+      <c r="CK1" s="1" t="inlineStr">
         <is>
           <t>Triple Threat Jab Step</t>
         </is>
       </c>
-      <c r="BV1" s="1" t="inlineStr">
+      <c r="CL1" s="1" t="inlineStr">
         <is>
           <t>Triple Threat Pump Fake</t>
         </is>
       </c>
-      <c r="BW1" s="1" t="inlineStr">
+      <c r="CM1" s="1" t="inlineStr">
+        <is>
+          <t>Triple Threat Shoot</t>
+        </is>
+      </c>
+      <c r="CN1" s="1" t="inlineStr">
         <is>
           <t>Use Glass</t>
         </is>
@@ -2437,7 +2519,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DS1"/>
+  <dimension ref="A1:DT1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2473,590 +2555,595 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Ankle Assassin</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Ankle Breaker</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>ANKLE_BRACES</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Ankle Breaker</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>BACKDOWN_PUNISHER</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Bail Out</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>BALL_STRIPPER</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>BLINDERS</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>BOX</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Boxout Beast</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Break Starter</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Brick Wall</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>BULLET_PASSER</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>BULLY</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>CATCH_SHOOT</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Challenger</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>CHASE_DOWN_ARTIST</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>CHEF</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>CIRCUS_THREES</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>CLAMPS</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>CLAMP_BREAKER</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>CLAMPS</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>CLAYMORE</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>CLUTCH_SHOOTER</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>COMEBACK_KID</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>CORNER_SPECIALIST</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Deadeye</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>DEFENSIVE_LEADER</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>DIFFICULT_SHOTS</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Dimer</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>DOWNHILL</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>DREAM_SHAKE</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>DROP-STEPPER</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>FADE_ACE</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>FAST_TWITCH</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>FEARLESS_FINISHER</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Float Game</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>FLOOR_GENERAL</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>GIANT_SLAYER</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Glove</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>GLUE_HANDS</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>GRACE_UNDER_PRESSURE</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>GREEN_MACHINE</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>GUARD_UP</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
-        <is>
-          <t>Handles For Days</t>
-        </is>
-      </c>
       <c r="AV1" s="1" t="inlineStr">
         <is>
-          <t>High Flying Denier</t>
+          <t>Handles for Days</t>
         </is>
       </c>
       <c r="AW1" s="1" t="inlineStr">
         <is>
+          <t>High-Flying Denier</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
           <t>HIGH_WORK_ETHIC</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>Hook Specialist</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>HOT_ZONE_HUNTER</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>HUSTLER</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>HYPERDRIVE</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>Immovable Enforcer</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>Interceptor</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>INTIMIDATOR</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>KILLER_COMBOS</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>Layup Mixmaster</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>LEGENDARY_WORK_ETHIC</t>
         </is>
       </c>
-      <c r="BH1" s="1" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>Lightning Launch</t>
         </is>
       </c>
-      <c r="BI1" s="1" t="inlineStr">
+      <c r="BJ1" s="1" t="inlineStr">
         <is>
           <t>Limitless Range</t>
         </is>
       </c>
-      <c r="BJ1" s="1" t="inlineStr">
+      <c r="BK1" s="1" t="inlineStr">
         <is>
           <t>LIMITLESS_SPOT-UP</t>
         </is>
       </c>
-      <c r="BK1" s="1" t="inlineStr">
+      <c r="BL1" s="1" t="inlineStr">
         <is>
           <t>LIMITLESS_TAKEOFF</t>
         </is>
       </c>
-      <c r="BL1" s="1" t="inlineStr">
+      <c r="BM1" s="1" t="inlineStr">
         <is>
           <t>LOB_CITY_FINISHER</t>
         </is>
       </c>
-      <c r="BM1" s="1" t="inlineStr">
+      <c r="BN1" s="1" t="inlineStr">
         <is>
           <t>LUCKY7</t>
         </is>
       </c>
-      <c r="BN1" s="1" t="inlineStr">
+      <c r="BO1" s="1" t="inlineStr">
         <is>
           <t>Marketability</t>
         </is>
       </c>
-      <c r="BO1" s="1" t="inlineStr">
+      <c r="BP1" s="1" t="inlineStr">
         <is>
           <t>MASHER</t>
         </is>
       </c>
-      <c r="BP1" s="1" t="inlineStr">
+      <c r="BQ1" s="1" t="inlineStr">
         <is>
           <t>MENACE</t>
         </is>
       </c>
-      <c r="BQ1" s="1" t="inlineStr">
+      <c r="BR1" s="1" t="inlineStr">
         <is>
           <t>MIDDY_MAGICIAN</t>
         </is>
       </c>
-      <c r="BR1" s="1" t="inlineStr">
+      <c r="BS1" s="1" t="inlineStr">
         <is>
           <t>Mini Marksman</t>
         </is>
       </c>
-      <c r="BS1" s="1" t="inlineStr">
+      <c r="BT1" s="1" t="inlineStr">
         <is>
           <t>MISMATCH_EXPERT</t>
         </is>
       </c>
-      <c r="BT1" s="1" t="inlineStr">
+      <c r="BU1" s="1" t="inlineStr">
         <is>
           <t>MOTIVATOR</t>
         </is>
       </c>
-      <c r="BU1" s="1" t="inlineStr">
+      <c r="BV1" s="1" t="inlineStr">
         <is>
           <t>MOUSE_IN_THE_HOUSE</t>
         </is>
       </c>
-      <c r="BV1" s="1" t="inlineStr">
+      <c r="BW1" s="1" t="inlineStr">
         <is>
           <t>NEEDLE_THREADER</t>
         </is>
       </c>
-      <c r="BW1" s="1" t="inlineStr">
-        <is>
-          <t>Off Ball Pest</t>
-        </is>
-      </c>
       <c r="BX1" s="1" t="inlineStr">
         <is>
-          <t>On Ball Menace</t>
+          <t>Off-Ball Pest</t>
         </is>
       </c>
       <c r="BY1" s="1" t="inlineStr">
         <is>
+          <t>On-Ball Menace</t>
+        </is>
+      </c>
+      <c r="BZ1" s="1" t="inlineStr">
+        <is>
           <t>Paint Patroller</t>
         </is>
       </c>
-      <c r="BZ1" s="1" t="inlineStr">
+      <c r="CA1" s="1" t="inlineStr">
         <is>
           <t>Paint Prodigy</t>
         </is>
       </c>
-      <c r="CA1" s="1" t="inlineStr">
+      <c r="CB1" s="1" t="inlineStr">
         <is>
           <t>Physical Finisher</t>
         </is>
       </c>
-      <c r="CB1" s="1" t="inlineStr">
+      <c r="CC1" s="1" t="inlineStr">
         <is>
           <t>PHYTHM_SHOOTER</t>
         </is>
       </c>
-      <c r="CC1" s="1" t="inlineStr">
+      <c r="CD1" s="1" t="inlineStr">
         <is>
           <t>Pick Dodger</t>
         </is>
       </c>
-      <c r="CD1" s="1" t="inlineStr">
+      <c r="CE1" s="1" t="inlineStr">
         <is>
           <t>PICK_POCKET</t>
         </is>
       </c>
-      <c r="CE1" s="1" t="inlineStr">
+      <c r="CF1" s="1" t="inlineStr">
         <is>
           <t>Pogo Stick</t>
         </is>
       </c>
-      <c r="CF1" s="1" t="inlineStr">
+      <c r="CG1" s="1" t="inlineStr">
+        <is>
+          <t>Post Fade Phenom</t>
+        </is>
+      </c>
+      <c r="CH1" s="1" t="inlineStr">
+        <is>
+          <t>Post Lockdown</t>
+        </is>
+      </c>
+      <c r="CI1" s="1" t="inlineStr">
+        <is>
+          <t>Post Powerhouse</t>
+        </is>
+      </c>
+      <c r="CJ1" s="1" t="inlineStr">
+        <is>
+          <t>Post-Up Poet</t>
+        </is>
+      </c>
+      <c r="CK1" s="1" t="inlineStr">
         <is>
           <t>Posterizer</t>
         </is>
       </c>
-      <c r="CG1" s="1" t="inlineStr">
-        <is>
-          <t>Post Fade Phenom</t>
-        </is>
-      </c>
-      <c r="CH1" s="1" t="inlineStr">
-        <is>
-          <t>Post Lockdown</t>
-        </is>
-      </c>
-      <c r="CI1" s="1" t="inlineStr">
+      <c r="CL1" s="1" t="inlineStr">
         <is>
           <t>POST_PLAYMAKER</t>
         </is>
       </c>
-      <c r="CJ1" s="1" t="inlineStr">
-        <is>
-          <t>Post Powerhouse</t>
-        </is>
-      </c>
-      <c r="CK1" s="1" t="inlineStr">
+      <c r="CM1" s="1" t="inlineStr">
         <is>
           <t>POST_SPIN_TECHNICIAN</t>
         </is>
       </c>
-      <c r="CL1" s="1" t="inlineStr">
-        <is>
-          <t>Post Up Poet</t>
-        </is>
-      </c>
-      <c r="CM1" s="1" t="inlineStr">
+      <c r="CN1" s="1" t="inlineStr">
         <is>
           <t>PRO_TOUCH</t>
         </is>
       </c>
-      <c r="CN1" s="1" t="inlineStr">
+      <c r="CO1" s="1" t="inlineStr">
         <is>
           <t>PUTBACK_BOSS</t>
         </is>
       </c>
-      <c r="CO1" s="1" t="inlineStr">
+      <c r="CP1" s="1" t="inlineStr">
         <is>
           <t>QUICK_CHAIN</t>
         </is>
       </c>
-      <c r="CP1" s="1" t="inlineStr">
+      <c r="CQ1" s="1" t="inlineStr">
         <is>
           <t>QUICK_FIRST_STEP</t>
         </is>
       </c>
-      <c r="CQ1" s="1" t="inlineStr">
+      <c r="CR1" s="1" t="inlineStr">
         <is>
           <t>Rebound Chaser</t>
         </is>
       </c>
-      <c r="CR1" s="1" t="inlineStr">
+      <c r="CS1" s="1" t="inlineStr">
         <is>
           <t>RIM_PROTECTOR</t>
         </is>
       </c>
-      <c r="CS1" s="1" t="inlineStr">
+      <c r="CT1" s="1" t="inlineStr">
         <is>
           <t>Rise Up</t>
         </is>
       </c>
-      <c r="CT1" s="1" t="inlineStr">
+      <c r="CU1" s="1" t="inlineStr">
+        <is>
+          <t>Set Shot Specialist</t>
+        </is>
+      </c>
+      <c r="CV1" s="1" t="inlineStr">
         <is>
           <t>SET_SHOOTER</t>
         </is>
       </c>
-      <c r="CU1" s="1" t="inlineStr">
-        <is>
-          <t>Set Shot Specialist</t>
-        </is>
-      </c>
-      <c r="CV1" s="1" t="inlineStr">
+      <c r="CW1" s="1" t="inlineStr">
         <is>
           <t>Shifty Shooter</t>
         </is>
       </c>
-      <c r="CW1" s="1" t="inlineStr">
-        <is>
-          <t>Slippery Off Ball</t>
-        </is>
-      </c>
       <c r="CX1" s="1" t="inlineStr">
         <is>
+          <t>Slippery Off-Ball</t>
+        </is>
+      </c>
+      <c r="CY1" s="1" t="inlineStr">
+        <is>
           <t>SLITHERY</t>
         </is>
       </c>
-      <c r="CY1" s="1" t="inlineStr">
+      <c r="CZ1" s="1" t="inlineStr">
         <is>
           <t>SLITHERY_FINISHER</t>
         </is>
       </c>
-      <c r="CZ1" s="1" t="inlineStr">
+      <c r="DA1" s="1" t="inlineStr">
         <is>
           <t>SNIPER</t>
         </is>
       </c>
-      <c r="DA1" s="1" t="inlineStr">
+      <c r="DB1" s="1" t="inlineStr">
         <is>
           <t>SPACE_CREATOR</t>
         </is>
       </c>
-      <c r="DB1" s="1" t="inlineStr">
+      <c r="DC1" s="1" t="inlineStr">
         <is>
           <t>SPECIAL_DELIVERY</t>
         </is>
       </c>
-      <c r="DC1" s="1" t="inlineStr">
+      <c r="DD1" s="1" t="inlineStr">
         <is>
           <t>STOP_GO</t>
         </is>
       </c>
-      <c r="DD1" s="1" t="inlineStr">
+      <c r="DE1" s="1" t="inlineStr">
         <is>
           <t>STOP_POP</t>
         </is>
       </c>
-      <c r="DE1" s="1" t="inlineStr">
-        <is>
-          <t>Strong Handles</t>
-        </is>
-      </c>
       <c r="DF1" s="1" t="inlineStr">
         <is>
+          <t>Strong Handle</t>
+        </is>
+      </c>
+      <c r="DG1" s="1" t="inlineStr">
+        <is>
           <t>TEAR_DROPPER</t>
         </is>
       </c>
-      <c r="DG1" s="1" t="inlineStr">
+      <c r="DH1" s="1" t="inlineStr">
         <is>
           <t>TIGHT_HANDLES</t>
         </is>
       </c>
-      <c r="DH1" s="1" t="inlineStr">
+      <c r="DI1" s="1" t="inlineStr">
         <is>
           <t>TIRELESS_DEFENDER</t>
         </is>
       </c>
-      <c r="DI1" s="1" t="inlineStr">
+      <c r="DJ1" s="1" t="inlineStr">
         <is>
           <t>TRAILBLAZER</t>
         </is>
       </c>
-      <c r="DJ1" s="1" t="inlineStr">
+      <c r="DK1" s="1" t="inlineStr">
         <is>
           <t>TRIPLE_THREAT_JUKE</t>
         </is>
       </c>
-      <c r="DK1" s="1" t="inlineStr">
+      <c r="DL1" s="1" t="inlineStr">
         <is>
           <t>ULTIMATE_MOTIVATOR</t>
         </is>
       </c>
-      <c r="DL1" s="1" t="inlineStr">
+      <c r="DM1" s="1" t="inlineStr">
         <is>
           <t>ULTIMATE_TRAILBLAZER</t>
         </is>
       </c>
-      <c r="DM1" s="1" t="inlineStr">
+      <c r="DN1" s="1" t="inlineStr">
         <is>
           <t>Unpluckable</t>
         </is>
       </c>
-      <c r="DN1" s="1" t="inlineStr">
+      <c r="DO1" s="1" t="inlineStr">
         <is>
           <t>UNSTRIPPABLE</t>
         </is>
       </c>
-      <c r="DO1" s="1" t="inlineStr">
+      <c r="DP1" s="1" t="inlineStr">
         <is>
           <t>Versatile Visionary</t>
         </is>
       </c>
-      <c r="DP1" s="1" t="inlineStr">
+      <c r="DQ1" s="1" t="inlineStr">
         <is>
           <t>VICE_GRIP</t>
         </is>
       </c>
-      <c r="DQ1" s="1" t="inlineStr">
+      <c r="DR1" s="1" t="inlineStr">
         <is>
           <t>VOLUME_SHOOTER</t>
         </is>
       </c>
-      <c r="DR1" s="1" t="inlineStr">
+      <c r="DS1" s="1" t="inlineStr">
         <is>
           <t>WORK_HORSE</t>
         </is>
       </c>
-      <c r="DS1" s="1" t="inlineStr">
+      <c r="DT1" s="1" t="inlineStr">
         <is>
           <t>WORM</t>
         </is>
@@ -3169,7 +3256,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3180,105 +3267,70 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>MYPLAYER_CLOTHES_TYPE</t>
+          <t>Shoe Away</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>PREGAME_OUTFIT</t>
+          <t>Shoe Home</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>SHIRTS_ITEM_FREQUENCY</t>
+          <t>Shoe Locked Vendor (Broken)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Shoe Away</t>
+          <t>Shorts</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Shoe Away Colorway</t>
+          <t>Shorts Away Color</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Shoe Home</t>
+          <t>Shorts Frequency</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>SHOE_HOME_COLORWAY_ID</t>
+          <t>Shorts Home Color</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Shoe Locked Vendor (Broken)</t>
+          <t>Shorts Length</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Shorts</t>
+          <t>Shorts Preferred Type</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Shorts Away Color</t>
+          <t>Sock Length Away</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Shorts Home Color</t>
+          <t>Sock Length Home</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Shorts Length</t>
+          <t>Undershirt</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>SHORTS_PREFERRED_LENGTH</t>
+          <t>Undershirt Away Color</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Shorts Preferred Type</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>SOCK_COLOR_AWAY</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>SOCK_COLOR_HOME</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Sock Length Away</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Sock Length Home</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Undershirt</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Undershirt Away Color</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Undershirt Home Color</t>
         </is>
@@ -3295,7 +3347,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA1"/>
+  <dimension ref="A1:BE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3316,255 +3368,275 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Headband Frequency</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Headband Logo</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>HEADBAND_CUSTOM_COLOR</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Headband Frequency</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Headband Logo</t>
-        </is>
-      </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Is Leg Frequency Paired</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Knee Frequency Paired</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Left Ankle</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Left Ankle Item Away Color</t>
-        </is>
-      </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Left Ankle Item Home Color</t>
+          <t>Left Ankle Away Color</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>Left Ankle Home Color</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>Left Arm Frequency</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Left Arm Home Color</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Left Arm Item Away Color</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Left Arm Item Home Color</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Left Elbow</t>
-        </is>
-      </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Left Elbow Item Away Color</t>
+          <t>Left Elbow Away Color</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
+          <t>Left Elbow Frequency</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>Left Elbow Item Home Color</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Left Fingers</t>
-        </is>
-      </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Left Fingers Item Away Color</t>
+          <t>Left Fingers Away Color</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Left Fingers Item Home Colro</t>
+          <t>Left Fingers Frequency</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
+          <t>Left Fingers Home Color</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Left Fingers Item Home Color</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
           <t>Left Knee</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Left Knee Home Color</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Left Knee Item Away Color</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Left Knee Item Home Color</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Left Leg</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Left Leg Item Away Color</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Left Leg Item Home Color</t>
-        </is>
-      </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Left Wrist Frequency</t>
+          <t>Left Leg Away Color</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>Left Wrist Item Away Color</t>
+          <t>Left Leg Home Color</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>Left Wrist Item Home Color</t>
+          <t>Left Wrist</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>Leg Frequency Paired</t>
+          <t>Left Wrist Away Color</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
+          <t>Left Wrist Home Color</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
           <t>Right Ankle</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>Right Ankle Item Away Color</t>
-        </is>
-      </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
+          <t>Right Ankle Away Color</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
           <t>Right Ankle Item Home Color</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>Right Arm Frequency</t>
-        </is>
-      </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>Right Arm Item Away Color</t>
+          <t>Right Arm</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>Right Arm Item Home Color</t>
+          <t>Right Arm Away Color</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
+          <t>Right Arm Home Color</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
           <t>Right Elbow Frequency</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Right Elbow Home Color</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Right Elbow Item Away Color</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>Right Elbow Item Home Color</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Right Fingers Away Color</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Right Fingers Frequency</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>Right Fingers Item Away Color</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>Right Fingers Item Home Color</t>
-        </is>
-      </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
-          <t>Right Knee</t>
+          <t>Right Fingers Home Color</t>
         </is>
       </c>
       <c r="AP1" s="1" t="inlineStr">
         <is>
-          <t>Right Knee Item Away Color</t>
+          <t>Right Knee Away Color</t>
         </is>
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
+          <t>Right Knee Frequency</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
           <t>Right Knee Item Home Color</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>Right Leg Frequency</t>
-        </is>
-      </c>
       <c r="AS1" s="1" t="inlineStr">
         <is>
+          <t>Right Leg</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Right Leg Home Color</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
           <t>Right Leg Item Away Color</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
-        <is>
-          <t>Right Leg Item Home Color</t>
-        </is>
-      </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>Right Wrist Away Color</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>Right Wrist Frequency</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
-        <is>
-          <t>Right Wrist Item Away Color</t>
-        </is>
-      </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>Right Wrist Item Home Color</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>Shorts</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>Shorts Away Color</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
-        <is>
-          <t>Shorts Frequency</t>
-        </is>
-      </c>
       <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>Shorts Compression</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>Shorts Compression Away Color</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>Shorts Compression Frequency</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>Shorts Compression Home Color</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>Shorts Home Color</t>
         </is>
@@ -3581,7 +3653,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3592,50 +3664,75 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Three Right Center</t>
+          <t>CENTER_3</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Three Left Center</t>
+          <t>Close Left</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Close Middle</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Close Right</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>LEFT_3</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Mid Range Left Center</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Mid-Range Right</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Mid-Range Right-Center</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>RIGHT_3</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Three Center</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Three Left</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Three Left-Center</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>Three Right</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Close Left</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Close Middle</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Close Right</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Mid Range Right Center</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Mid Range Left</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Mid Range Right</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Three Right-Center</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Under Basket</t>
         </is>
@@ -3652,7 +3749,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BF1"/>
+  <dimension ref="A1:BG1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3703,7 +3800,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Dribble Pull Up</t>
+          <t>Dribble Pull-Up</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -3798,155 +3895,160 @@
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
+          <t>Go-To Dunk Package</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Go-To Shot</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Hop Jumper</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Jumpball Ritual</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Jumpshot Base</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Jumpshot Blending</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Layup Package</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Lower/Base</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Motion Style</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Moving Behind The Back</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Moving Crossover</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Moving Hesitation</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Moving Spin</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Moving Stepback</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Pass Style</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Post Fade</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
           <t>Post Go-To Shot</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>Go To Dunk Package</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>Go To Shot</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>Hop Jumper</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Post Hook</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>Post Hop Shot</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>Jumpball Ritual</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>Layup Package</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>Lower/Base</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>Motion Style</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>Moving Behind The Back</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
-        <is>
-          <t>Moving Crossover</t>
-        </is>
-      </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>Moving Hesitation</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>Moving Spin</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>Moving Stepback</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>NBA Jumpball Ritual</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>Pass Style</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>Post Fade</t>
-        </is>
-      </c>
-      <c r="AS1" s="1" t="inlineStr">
-        <is>
-          <t>Post Hook</t>
-        </is>
-      </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>Post Spin Shot</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>Post Spin Spot</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
-        <is>
-          <t>Pre Game 1</t>
-        </is>
-      </c>
       <c r="AW1" s="1" t="inlineStr">
         <is>
-          <t>Pre Game 2</t>
+          <t>Pre-Game 1</t>
         </is>
       </c>
       <c r="AX1" s="1" t="inlineStr">
         <is>
+          <t>Pre-Game 2</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
           <t>Regular Breakdown Combos</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>Release Timing</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>Signature Size-Up</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>SIGNATURE_COMBOS</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
-        <is>
-          <t>Signature Size Up</t>
-        </is>
-      </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>SIZE-UP_ESCAPE_PACKAGES</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>Spin Jumper</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>Triple Threat Style</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>Upper Release 1</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>Upper Release 2</t>
         </is>

</xml_diff>